<commit_message>
update clp format for empty bone animation
</commit_message>
<xml_diff>
--- a/doc/CLP.xlsx
+++ b/doc/CLP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n_seh\source\repos\Project4E53\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n_seh\source\repos\modelconvert\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A673BB67-D5EA-4B86-826C-D5CD7315F0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DAC20B-20E9-473E-9BC0-B4A608F701BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D5EF262-ECCE-4192-ADE7-EFB17208BE4A}"/>
   </bookViews>
@@ -97,7 +97,7 @@
     <t>repeat for every bone</t>
   </si>
   <si>
-    <t>repeat for every key frame</t>
+    <t>repeat for every key frame / if -1 no keyframe and skip to next</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
     <col min="3" max="3" width="3.140625" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="6" max="6" width="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">

</xml_diff>